<commit_message>
Adding Program Delete feature and step definition and Put feature files
</commit_message>
<xml_diff>
--- a/src/test/resources/excelData/program_testdata.xlsx
+++ b/src/test/resources/excelData/program_testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ranjith\SangNewWorkspace\7CRUDCarriers_LMS_API\src\test\resources\excelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6742210F-6EBB-4CDF-A964-B74F12062533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E149A90-6822-4330-95BE-ACD4363AD3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="3705" windowWidth="15330" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="get" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="81">
   <si>
     <t>Test case Name</t>
   </si>
@@ -100,19 +100,7 @@
     <t>To update visa status with invalid input</t>
   </si>
   <si>
-    <t>To delete the user id with existing user id</t>
-  </si>
-  <si>
     <t>404</t>
-  </si>
-  <si>
-    <t>Not Found</t>
-  </si>
-  <si>
-    <t>To delete the user with invalid user id</t>
-  </si>
-  <si>
-    <t>U72</t>
   </si>
   <si>
     <t>1.23</t>
@@ -162,15 +150,6 @@
   </si>
   <si>
     <t>User Successfully Updated</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>To delete the user id with non-existing user id</t>
-  </si>
-  <si>
-    <t>Deleted</t>
   </si>
   <si>
     <t>{
@@ -422,9 +401,6 @@
 }</t>
   </si>
   <si>
-    <t>U156</t>
-  </si>
-  <si>
     <t>ProgramId</t>
   </si>
   <si>
@@ -453,13 +429,46 @@
   </si>
   <si>
     <t>Null</t>
+  </si>
+  <si>
+    <t>To delete existing program by id</t>
+  </si>
+  <si>
+    <t>To delete existing program by name</t>
+  </si>
+  <si>
+    <t>Deleted Successfully</t>
+  </si>
+  <si>
+    <t>Bad Request</t>
+  </si>
+  <si>
+    <t>Not found</t>
+  </si>
+  <si>
+    <t>To delete non-existing program by id</t>
+  </si>
+  <si>
+    <t>To delete non-existing program by name</t>
+  </si>
+  <si>
+    <t>6000</t>
+  </si>
+  <si>
+    <t>Java267</t>
+  </si>
+  <si>
+    <t>To delete the program without passing the program id or name</t>
+  </si>
+  <si>
+    <t>Java270</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,6 +483,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0451A5"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -490,7 +511,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -513,11 +534,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -552,6 +586,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -830,14 +873,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -846,7 +889,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>8</v>
@@ -854,7 +897,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>9</v>
@@ -862,7 +905,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B3" s="12">
         <v>520</v>
@@ -873,10 +916,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>13</v>
@@ -884,10 +927,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>13</v>
@@ -895,10 +938,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>13</v>
@@ -906,10 +949,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>13</v>
@@ -917,7 +960,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>13</v>
@@ -927,7 +970,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C2:C8 B4 B7" numberStoredAsText="1"/>
+    <ignoredError sqref="C2 B7 C4:C8 B4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -967,21 +1010,21 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
@@ -992,10 +1035,10 @@
     </row>
     <row r="4" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
@@ -1009,7 +1052,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>13</v>
@@ -1023,7 +1066,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -1037,13 +1080,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -1051,7 +1094,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>13</v>
@@ -1065,7 +1108,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>13</v>
@@ -1079,7 +1122,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>13</v>
@@ -1093,7 +1136,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>13</v>
@@ -1104,10 +1147,10 @@
     </row>
     <row r="12" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>13</v>
@@ -1118,16 +1161,16 @@
     </row>
     <row r="13" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1175,16 +1218,16 @@
         <v>15</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="225" x14ac:dyDescent="0.25">
@@ -1192,16 +1235,16 @@
         <v>17</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="240" x14ac:dyDescent="0.25">
@@ -1209,10 +1252,10 @@
         <v>19</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>13</v>
@@ -1226,16 +1269,16 @@
         <v>21</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="210" x14ac:dyDescent="0.25">
@@ -1243,16 +1286,16 @@
         <v>20</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="210" x14ac:dyDescent="0.25">
@@ -1260,10 +1303,10 @@
         <v>22</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>13</v>
@@ -1277,16 +1320,16 @@
         <v>23</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="240" x14ac:dyDescent="0.25">
@@ -1294,10 +1337,10 @@
         <v>24</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>13</v>
@@ -1316,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,72 +1369,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>67</v>
+      <c r="A2" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1883</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>29</v>
+      <c r="A3" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>39</v>
+      <c r="A4" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A5" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="C6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
@@ -1413,5 +1470,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>